<commit_message>
add to e2e tests
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/resources.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BBB2D6-5685-3A4C-8D9A-321CDDA6290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC174CA-3B0B-E247-AE80-B5B345C941E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34340" yWindow="5260" windowWidth="33600" windowHeight="20480" activeTab="1" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="-38400" yWindow="5260" windowWidth="33600" windowHeight="20480" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -1120,7 +1120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="140">
   <si>
     <t>Cardinality</t>
   </si>
@@ -1532,6 +1532,15 @@
   </si>
   <si>
     <t>label_de</t>
+  </si>
+  <si>
+    <t>NoCardinalityClass</t>
+  </si>
+  <si>
+    <t>Class Without Cardinalities</t>
+  </si>
+  <si>
+    <t>No cardinalitiy</t>
   </si>
 </sst>
 </file>
@@ -2007,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7011A-D3D9-4EA8-AB3C-BA62FE335401}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2386,13 +2395,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
       </c>
       <c r="C13" t="s">
         <v>91</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="H13" t="s">
         <v>90</v>
@@ -2401,7 +2413,7 @@
         <v>91</v>
       </c>
       <c r="L13" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -2557,7 +2569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>

</xml_diff>

<commit_message>
feat(excel2json): creating classes without any cardinalities (DEV-3755) (#1029)
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/resources.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2json_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF51E70-ECAC-9F44-A357-6C4549DE8259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC174CA-3B0B-E247-AE80-B5B345C941E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="-38400" yWindow="5260" windowWidth="33600" windowHeight="20480" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1121,7 +1120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="140">
   <si>
     <t>Cardinality</t>
   </si>
@@ -1438,9 +1437,6 @@
     <t>PDF-Dokument</t>
   </si>
   <si>
-    <t>invalid</t>
-  </si>
-  <si>
     <t xml:space="preserve">             </t>
   </si>
   <si>
@@ -1536,6 +1532,15 @@
   </si>
   <si>
     <t>label_de</t>
+  </si>
+  <si>
+    <t>NoCardinalityClass</t>
+  </si>
+  <si>
+    <t>Class Without Cardinalities</t>
+  </si>
+  <si>
+    <t>No cardinalitiy</t>
   </si>
 </sst>
 </file>
@@ -2012,7 +2017,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2033,19 +2038,19 @@
         <v>17</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>134</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>60</v>
@@ -2060,7 +2065,7 @@
         <v>63</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>18</v>
@@ -2089,25 +2094,25 @@
         <v>65</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
         <v>124</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>125</v>
-      </c>
-      <c r="I2" t="s">
-        <v>126</v>
       </c>
       <c r="J2" t="s">
         <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M2" t="s">
         <v>91</v>
@@ -2133,10 +2138,10 @@
         <v>66</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>101</v>
@@ -2162,10 +2167,10 @@
         <v>67</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L4" t="s">
         <v>100</v>
@@ -2191,13 +2196,13 @@
         <v>68</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N5" t="s">
         <v>90</v>
@@ -2220,10 +2225,10 @@
         <v>99</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>19</v>
@@ -2246,10 +2251,10 @@
         <v>98</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L7" t="s">
         <v>19</v>
@@ -2266,7 +2271,7 @@
         <v>74</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="6"/>
       <c r="G8" t="s">
@@ -2276,7 +2281,7 @@
         <v>75</v>
       </c>
       <c r="L8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2285,7 +2290,7 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
         <v>91</v>
@@ -2319,7 +2324,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
         <v>91</v>
@@ -2345,10 +2350,10 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G11" t="s">
         <v>80</v>
@@ -2370,7 +2375,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>103</v>
@@ -2390,13 +2395,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
       </c>
       <c r="C13" t="s">
         <v>91</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="H13" t="s">
         <v>90</v>
@@ -2405,7 +2413,7 @@
         <v>91</v>
       </c>
       <c r="L13" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -2413,10 +2421,10 @@
         <v>90</v>
       </c>
       <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
         <v>108</v>
-      </c>
-      <c r="E14" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -2424,31 +2432,31 @@
         <v>91</v>
       </c>
       <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" t="s">
         <v>107</v>
-      </c>
-      <c r="L15" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
         <v>91</v>
       </c>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.2">
       <c r="I18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2559,11 +2567,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2581,12 +2589,12 @@
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -2597,7 +2605,7 @@
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -2608,7 +2616,7 @@
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -2622,7 +2630,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -2633,7 +2641,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="3">
         <v>4</v>
@@ -2644,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
@@ -2706,59 +2714,47 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="3">
-        <v>11</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
       </c>
       <c r="C14" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>107</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2792,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2941,7 +2937,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2957,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -3181,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3222,7 +3218,7 @@
         <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -3256,7 +3252,7 @@
         <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -3324,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3365,7 +3361,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix(excel2json): enable references to other ontologies in resource cardinalities (DEV-5416) (#1954)
</commit_message>
<xml_diff>
--- a/testdata/excel2json/excel2json_files/test-name (test_label)/resources.xlsx
+++ b/testdata/excel2json/excel2json_files/test-name (test_label)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/excel2json_files/test-name (test_label)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CDF264-5B1F-1848-914B-39DABAF8917A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23CFADD-2CC4-3848-9AD8-51F2E3A9BA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="7" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -1120,7 +1120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="146">
   <si>
     <t>Cardinality</t>
   </si>
@@ -1550,6 +1550,15 @@
   </si>
   <si>
     <t>default_permissions_overrule</t>
+  </si>
+  <si>
+    <t>other-onto:hasProp</t>
+  </si>
+  <si>
+    <t>seqnum</t>
+  </si>
+  <si>
+    <t>isPartOf</t>
   </si>
 </sst>
 </file>
@@ -1727,9 +1736,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1767,7 +1776,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1873,7 +1882,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2015,7 +2024,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2025,7 +2034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7011A-D3D9-4EA8-AB3C-BA62FE335401}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -2584,7 +2593,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2765,9 +2774,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>54</v>
+      </c>
+      <c r="C17" s="4">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3583,10 +3598,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D91115-9643-C84D-8DE4-4276C702C3EC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3605,6 +3620,22 @@
       </c>
       <c r="B2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>